<commit_message>
Fix API Question payload data structure to match React QuestionView expected data structure
</commit_message>
<xml_diff>
--- a/backend/API Design.xlsx
+++ b/backend/API Design.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bnik/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bnik/code/trivia_quizzes/backend/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{383A6B24-919C-D24F-89A2-1ABCF445BE6C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{420AB00A-E59D-1F42-8372-32AD1969FC43}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="13420" windowWidth="33600" windowHeight="7580" activeTab="1" xr2:uid="{6337297E-AEAA-7D4F-921E-C16E187DF1E1}"/>
+    <workbookView xWindow="460" yWindow="-13100" windowWidth="28800" windowHeight="11300" activeTab="1" xr2:uid="{6337297E-AEAA-7D4F-921E-C16E187DF1E1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="44">
   <si>
     <t>Endpoint</t>
   </si>
@@ -161,6 +161,9 @@
   </si>
   <si>
     <t>Search</t>
+  </si>
+  <si>
+    <t>201,</t>
   </si>
 </sst>
 </file>
@@ -176,12 +179,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -196,7 +205,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -214,6 +223,16 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -533,7 +552,7 @@
   <dimension ref="B6:G17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6:G7"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -682,7 +701,7 @@
   <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -690,8 +709,7 @@
     <col min="1" max="1" width="32.83203125" style="2" customWidth="1"/>
     <col min="2" max="2" width="6" style="1" customWidth="1"/>
     <col min="3" max="3" width="31.83203125" customWidth="1"/>
-    <col min="4" max="4" width="8.33203125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="8.33203125" customWidth="1"/>
+    <col min="4" max="5" width="8.33203125" style="1" customWidth="1"/>
     <col min="6" max="7" width="10" style="6" customWidth="1"/>
     <col min="8" max="9" width="8.33203125" customWidth="1"/>
     <col min="10" max="10" width="18.1640625" customWidth="1"/>
@@ -739,24 +757,35 @@
       <c r="D2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="1"/>
+      <c r="E2" s="1" t="s">
+        <v>9</v>
+      </c>
       <c r="F2" s="5"/>
       <c r="G2" s="5"/>
       <c r="J2" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
+    <row r="3" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="C3" t="s">
+      <c r="B3" s="8"/>
+      <c r="C3" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D3" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="J3" t="s">
+      <c r="E3" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="F3" s="10"/>
+      <c r="G3" s="10"/>
+      <c r="H3" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="J3" s="9" t="s">
         <v>26</v>
       </c>
     </row>

</xml_diff>

<commit_message>
/questions POST - Adding a single question
</commit_message>
<xml_diff>
--- a/backend/API Design.xlsx
+++ b/backend/API Design.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bnik/code/trivia_quizzes/backend/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{420AB00A-E59D-1F42-8372-32AD1969FC43}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA8AFF5D-269C-2446-A7FC-2C4E949AF7CD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="460" yWindow="-13100" windowWidth="28800" windowHeight="11300" activeTab="1" xr2:uid="{6337297E-AEAA-7D4F-921E-C16E187DF1E1}"/>
+    <workbookView xWindow="-5160" yWindow="-7940" windowWidth="38380" windowHeight="7940" activeTab="1" xr2:uid="{6337297E-AEAA-7D4F-921E-C16E187DF1E1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="52">
   <si>
     <t>Endpoint</t>
   </si>
@@ -148,9 +148,6 @@
     <t>list questions</t>
   </si>
   <si>
-    <t>search</t>
-  </si>
-  <si>
     <t>QuestionView</t>
   </si>
   <si>
@@ -160,10 +157,37 @@
     <t>/quizzes</t>
   </si>
   <si>
-    <t>Search</t>
-  </si>
-  <si>
-    <t>201,</t>
+    <t>delete a question</t>
+  </si>
+  <si>
+    <t>/questions/id</t>
+  </si>
+  <si>
+    <t>QuestionView questionAction</t>
+  </si>
+  <si>
+    <t>400, 404</t>
+  </si>
+  <si>
+    <t>/questions/search</t>
+  </si>
+  <si>
+    <t>search questions</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>json</t>
+  </si>
+  <si>
+    <t>Request body (if any)</t>
+  </si>
+  <si>
+    <t>Successful response body (if any)</t>
+  </si>
+  <si>
+    <t>POSTMAN TEST</t>
   </si>
 </sst>
 </file>
@@ -179,7 +203,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -189,6 +213,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -205,7 +235,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -234,6 +264,22 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -698,24 +744,26 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44CC1864-4D91-3A47-8904-26FEECCF1FBD}">
-  <dimension ref="A1:J9"/>
+  <dimension ref="A1:N9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="O1" sqref="O1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="32.83203125" style="2" customWidth="1"/>
     <col min="2" max="2" width="6" style="1" customWidth="1"/>
-    <col min="3" max="3" width="31.83203125" customWidth="1"/>
-    <col min="4" max="5" width="8.33203125" style="1" customWidth="1"/>
-    <col min="6" max="7" width="10" style="6" customWidth="1"/>
-    <col min="8" max="9" width="8.33203125" customWidth="1"/>
-    <col min="10" max="10" width="18.1640625" customWidth="1"/>
+    <col min="3" max="4" width="8.33203125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="31.83203125" customWidth="1"/>
+    <col min="6" max="8" width="10" style="6" customWidth="1"/>
+    <col min="9" max="9" width="10" style="5" customWidth="1"/>
+    <col min="10" max="10" width="8.33203125" style="1" customWidth="1"/>
+    <col min="11" max="11" width="12.83203125" style="1" customWidth="1"/>
+    <col min="12" max="12" width="18.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="4" customFormat="1" ht="46" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" s="4" customFormat="1" ht="72" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>18</v>
       </c>
@@ -723,13 +771,13 @@
         <v>32</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>1</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F1" s="3" t="s">
         <v>30</v>
@@ -738,143 +786,213 @@
         <v>34</v>
       </c>
       <c r="H1" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="J1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="K1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="L1" s="3" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="N1" s="4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C2" t="s">
-        <v>24</v>
+      <c r="C2" s="1" t="s">
+        <v>9</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="1" t="s">
-        <v>9</v>
+      <c r="E2" t="s">
+        <v>24</v>
       </c>
       <c r="F2" s="5"/>
       <c r="G2" s="5"/>
-      <c r="J2" t="s">
+      <c r="H2" s="5"/>
+      <c r="L2" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:14" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="7" t="s">
         <v>28</v>
       </c>
       <c r="B3" s="8"/>
-      <c r="C3" s="9" t="s">
-        <v>27</v>
+      <c r="C3" s="8" t="s">
+        <v>7</v>
       </c>
       <c r="D3" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="F3" s="10"/>
-      <c r="G3" s="10"/>
-      <c r="H3" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="J3" s="9" t="s">
+      <c r="E3" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="F3" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="G3" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="H3" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="I3" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="J3" s="8">
+        <v>201</v>
+      </c>
+      <c r="K3" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="L3" s="9" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>36</v>
       </c>
       <c r="B4" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="C4" t="s">
-        <v>33</v>
-      </c>
       <c r="D4" s="1" t="s">
         <v>8</v>
       </c>
+      <c r="E4" t="s">
+        <v>33</v>
+      </c>
       <c r="G4" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="J4" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="L4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>37</v>
       </c>
       <c r="B5" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="C5" t="s">
-        <v>27</v>
-      </c>
       <c r="D5" s="1" t="s">
         <v>8</v>
       </c>
+      <c r="E5" t="s">
+        <v>27</v>
+      </c>
       <c r="F5" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="J5" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A6" s="2" t="s">
+      <c r="L5" t="s">
         <v>38</v>
       </c>
-      <c r="C6" t="s">
-        <v>27</v>
-      </c>
-      <c r="D6" s="1" t="s">
+    </row>
+    <row r="6" spans="1:14" s="14" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="B6" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="C6" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="J6" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="C7" t="s">
-        <v>24</v>
-      </c>
+      <c r="E6" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="F6" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="G6" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="H6" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="I6" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="J6" s="13">
+        <v>205</v>
+      </c>
+      <c r="K6" s="13">
+        <v>400</v>
+      </c>
+      <c r="L6" s="14" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="D7" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J7" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="C8" t="s">
-        <v>41</v>
-      </c>
+      <c r="E7" t="s">
+        <v>24</v>
+      </c>
+      <c r="L7" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="D8" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="J8" t="s">
+      <c r="E8" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="J9" t="s">
+      <c r="L8" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A9" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E9" t="s">
         <v>42</v>
       </c>
+      <c r="H9" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="I9" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="J9" s="1">
+        <v>204</v>
+      </c>
+      <c r="K9" s="1">
+        <v>404</v>
+      </c>
+      <c r="L9" t="s">
+        <v>43</v>
+      </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J11">
-    <sortCondition ref="J2:J11"/>
-    <sortCondition ref="C2:C11"/>
-    <sortCondition ref="D2:D11"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:L11">
+    <sortCondition ref="L2:L11"/>
+    <sortCondition ref="E2:E11"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
test: /questions POST - Searching question
</commit_message>
<xml_diff>
--- a/backend/API Design.xlsx
+++ b/backend/API Design.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bnik/code/trivia_quizzes/backend/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA8AFF5D-269C-2446-A7FC-2C4E949AF7CD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74FEADE3-513E-7E46-A409-A464B16A77D8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-5160" yWindow="-7940" windowWidth="38380" windowHeight="7940" activeTab="1" xr2:uid="{6337297E-AEAA-7D4F-921E-C16E187DF1E1}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="58">
   <si>
     <t>Endpoint</t>
   </si>
@@ -145,9 +145,6 @@
     <t>list questions by category</t>
   </si>
   <si>
-    <t>list questions</t>
-  </si>
-  <si>
     <t>QuestionView</t>
   </si>
   <si>
@@ -169,12 +166,6 @@
     <t>400, 404</t>
   </si>
   <si>
-    <t>/questions/search</t>
-  </si>
-  <si>
-    <t>search questions</t>
-  </si>
-  <si>
     <t>-</t>
   </si>
   <si>
@@ -188,6 +179,33 @@
   </si>
   <si>
     <t>POSTMAN TEST</t>
+  </si>
+  <si>
+    <t>d/u Tests</t>
+  </si>
+  <si>
+    <t>Frontend Test</t>
+  </si>
+  <si>
+    <t>Git</t>
+  </si>
+  <si>
+    <t>list all questions with pagination</t>
+  </si>
+  <si>
+    <t>list search result questions with pagination</t>
+  </si>
+  <si>
+    <t>searchTerm</t>
+  </si>
+  <si>
+    <t>request body keys</t>
+  </si>
+  <si>
+    <t>expecting body keys</t>
+  </si>
+  <si>
+    <t>questions, total_questions, current_category</t>
   </si>
 </sst>
 </file>
@@ -744,26 +762,27 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44CC1864-4D91-3A47-8904-26FEECCF1FBD}">
-  <dimension ref="A1:N9"/>
+  <dimension ref="A1:T9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O1" sqref="O1"/>
+      <selection activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="32.83203125" style="2" customWidth="1"/>
+    <col min="1" max="1" width="49.33203125" style="2" customWidth="1"/>
     <col min="2" max="2" width="6" style="1" customWidth="1"/>
     <col min="3" max="4" width="8.33203125" style="1" customWidth="1"/>
     <col min="5" max="5" width="31.83203125" customWidth="1"/>
     <col min="6" max="8" width="10" style="6" customWidth="1"/>
-    <col min="9" max="9" width="10" style="5" customWidth="1"/>
-    <col min="10" max="10" width="8.33203125" style="1" customWidth="1"/>
-    <col min="11" max="11" width="12.83203125" style="1" customWidth="1"/>
-    <col min="12" max="12" width="18.1640625" customWidth="1"/>
+    <col min="9" max="9" width="13.6640625" style="6" customWidth="1"/>
+    <col min="10" max="11" width="10" style="5" customWidth="1"/>
+    <col min="12" max="12" width="8.33203125" style="1" customWidth="1"/>
+    <col min="13" max="13" width="12.83203125" style="1" customWidth="1"/>
+    <col min="14" max="14" width="18.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="4" customFormat="1" ht="72" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:20" s="4" customFormat="1" ht="72" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>18</v>
       </c>
@@ -786,25 +805,40 @@
         <v>34</v>
       </c>
       <c r="H1" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="P1" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q1" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="R1" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="J1" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="K1" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="L1" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="N1" s="4" t="s">
+      <c r="T1" s="4" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>29</v>
       </c>
@@ -820,11 +854,12 @@
       <c r="F2" s="5"/>
       <c r="G2" s="5"/>
       <c r="H2" s="5"/>
-      <c r="L2" t="s">
+      <c r="I2" s="5"/>
+      <c r="N2" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:14" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:20" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="7" t="s">
         <v>28</v>
       </c>
@@ -839,34 +874,33 @@
         <v>27</v>
       </c>
       <c r="F3" s="10" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="G3" s="10" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="H3" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="I3" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="J3" s="8">
+        <v>45</v>
+      </c>
+      <c r="I3" s="10"/>
+      <c r="J3" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="K3" s="11"/>
+      <c r="L3" s="8">
         <v>201</v>
       </c>
-      <c r="K3" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="L3" s="9" t="s">
+      <c r="M3" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="N3" s="9" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B4" s="1" t="b">
-        <v>0</v>
-      </c>
       <c r="D4" s="1" t="s">
         <v>8</v>
       </c>
@@ -876,13 +910,13 @@
       <c r="G4" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="L4" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="N4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>37</v>
+        <v>52</v>
       </c>
       <c r="B5" s="1" t="b">
         <v>1</v>
@@ -896,16 +930,16 @@
       <c r="F5" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="L5" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" s="14" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="N5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" s="14" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="12" t="s">
-        <v>46</v>
-      </c>
-      <c r="B6" s="13" t="s">
-        <v>47</v>
+        <v>53</v>
+      </c>
+      <c r="B6" s="13" t="b">
+        <v>1</v>
       </c>
       <c r="C6" s="13" t="s">
         <v>9</v>
@@ -914,55 +948,61 @@
         <v>6</v>
       </c>
       <c r="E6" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="F6" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="G6" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="H6" s="15" t="s">
         <v>45</v>
       </c>
-      <c r="F6" s="15" t="s">
-        <v>47</v>
-      </c>
-      <c r="G6" s="15" t="s">
-        <v>47</v>
-      </c>
-      <c r="H6" s="15" t="b">
+      <c r="I6" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="J6" s="16" t="b">
         <v>1</v>
       </c>
-      <c r="I6" s="16" t="b">
-        <v>1</v>
-      </c>
-      <c r="J6" s="13">
-        <v>205</v>
-      </c>
-      <c r="K6" s="13">
+      <c r="K6" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="L6" s="13">
+        <v>200</v>
+      </c>
+      <c r="M6" s="13">
         <v>400</v>
       </c>
-      <c r="L6" s="14" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="N6" s="14" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.2">
       <c r="D7" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E7" t="s">
         <v>24</v>
       </c>
-      <c r="L7" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="N7" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.2">
       <c r="D8" s="1" t="s">
         <v>6</v>
       </c>
       <c r="E8" t="s">
+        <v>39</v>
+      </c>
+      <c r="N8" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A9" s="2" t="s">
         <v>40</v>
-      </c>
-      <c r="L8" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A9" s="2" t="s">
-        <v>41</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>23</v>
@@ -971,29 +1011,30 @@
         <v>23</v>
       </c>
       <c r="E9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H9" s="6" t="b">
         <v>0</v>
       </c>
-      <c r="I9" s="5" t="b">
+      <c r="J9" s="5" t="b">
         <v>0</v>
       </c>
-      <c r="J9" s="1">
+      <c r="L9" s="1">
         <v>204</v>
       </c>
-      <c r="K9" s="1">
+      <c r="M9" s="1">
         <v>404</v>
       </c>
-      <c r="L9" t="s">
-        <v>43</v>
+      <c r="N9" t="s">
+        <v>42</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:L11">
-    <sortCondition ref="L2:L11"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:N11">
+    <sortCondition ref="N2:N11"/>
     <sortCondition ref="E2:E11"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
update endpoints in QuizView.js
</commit_message>
<xml_diff>
--- a/backend/API Design.xlsx
+++ b/backend/API Design.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bnik/code/trivia_quizzes/backend/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74FEADE3-513E-7E46-A409-A464B16A77D8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D0C3F82-D2A2-D048-9CD7-4626CD2056DA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-5160" yWindow="-7940" windowWidth="38380" windowHeight="7940" activeTab="1" xr2:uid="{6337297E-AEAA-7D4F-921E-C16E187DF1E1}"/>
+    <workbookView xWindow="0" yWindow="12460" windowWidth="33600" windowHeight="8540" activeTab="2" xr2:uid="{6337297E-AEAA-7D4F-921E-C16E187DF1E1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="trivia" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="73">
   <si>
     <t>Endpoint</t>
   </si>
@@ -142,9 +143,6 @@
     <t>id</t>
   </si>
   <si>
-    <t>list questions by category</t>
-  </si>
-  <si>
     <t>QuestionView</t>
   </si>
   <si>
@@ -202,10 +200,58 @@
     <t>request body keys</t>
   </si>
   <si>
-    <t>expecting body keys</t>
-  </si>
-  <si>
     <t>questions, total_questions, current_category</t>
+  </si>
+  <si>
+    <t>list/get questions based on category</t>
+  </si>
+  <si>
+    <t>frontend expecting body keys</t>
+  </si>
+  <si>
+    <t>/category/id/questions</t>
+  </si>
+  <si>
+    <t>Test, Code, Fail</t>
+  </si>
+  <si>
+    <t>Test</t>
+  </si>
+  <si>
+    <t>POSTMAN</t>
+  </si>
+  <si>
+    <t>Fail</t>
+  </si>
+  <si>
+    <t>Pass</t>
+  </si>
+  <si>
+    <t>Working on Tests</t>
+  </si>
+  <si>
+    <t>All Tests</t>
+  </si>
+  <si>
+    <t>Recode</t>
+  </si>
+  <si>
+    <t>/quizzes/categories</t>
+  </si>
+  <si>
+    <t>Read Docs Understanding Problem/Funcionality</t>
+  </si>
+  <si>
+    <t xml:space="preserve">undersranding existing data structuer </t>
+  </si>
+  <si>
+    <t>Framework Structure, TODOs, Hooks, SmallSteps, Placeholders</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>Correction, Redo</t>
   </si>
 </sst>
 </file>
@@ -230,13 +276,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.79998168889431442"/>
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -253,25 +299,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -281,10 +321,10 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -764,22 +804,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44CC1864-4D91-3A47-8904-26FEECCF1FBD}">
   <dimension ref="A1:T9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L6" sqref="L6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="49.33203125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="6" style="1" customWidth="1"/>
-    <col min="3" max="4" width="8.33203125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="31.83203125" customWidth="1"/>
-    <col min="6" max="8" width="10" style="6" customWidth="1"/>
-    <col min="9" max="9" width="13.6640625" style="6" customWidth="1"/>
-    <col min="10" max="11" width="10" style="5" customWidth="1"/>
-    <col min="12" max="12" width="8.33203125" style="1" customWidth="1"/>
-    <col min="13" max="13" width="12.83203125" style="1" customWidth="1"/>
-    <col min="14" max="14" width="18.1640625" customWidth="1"/>
+    <col min="1" max="1" width="49.33203125" style="5" customWidth="1"/>
+    <col min="2" max="2" width="6" style="6" customWidth="1"/>
+    <col min="3" max="4" width="8.33203125" style="6" customWidth="1"/>
+    <col min="5" max="5" width="31.83203125" style="7" customWidth="1"/>
+    <col min="6" max="8" width="10" style="9" customWidth="1"/>
+    <col min="9" max="9" width="13.6640625" style="9" customWidth="1"/>
+    <col min="10" max="10" width="10" style="8" customWidth="1"/>
+    <col min="11" max="11" width="19.5" style="8" customWidth="1"/>
+    <col min="12" max="12" width="8.33203125" style="6" customWidth="1"/>
+    <col min="13" max="13" width="12.83203125" style="6" customWidth="1"/>
+    <col min="14" max="14" width="18.1640625" style="7" customWidth="1"/>
+    <col min="15" max="16384" width="10.83203125" style="7"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20" s="4" customFormat="1" ht="72" customHeight="1" x14ac:dyDescent="0.2">
@@ -805,16 +847,16 @@
         <v>34</v>
       </c>
       <c r="H1" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="J1" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="I1" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>47</v>
-      </c>
       <c r="K1" s="3" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="L1" s="3" t="s">
         <v>3</v>
@@ -826,215 +868,426 @@
         <v>25</v>
       </c>
       <c r="P1" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="Q1" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="Q1" s="4" t="s">
+      <c r="R1" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="R1" s="4" t="s">
+      <c r="T1" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="T1" s="4" t="s">
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A2" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="F2" s="8"/>
+      <c r="G2" s="8"/>
+      <c r="H2" s="8"/>
+      <c r="I2" s="8"/>
+      <c r="N2" s="7" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A3" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="F3" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="G3" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="H3" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="J3" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="L3" s="6">
+        <v>201</v>
+      </c>
+      <c r="M3" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="N3" s="7" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="B4" s="11" t="b">
+        <v>1</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="F4" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="G4" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="H4" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="I4" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="J4" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="K4" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="L4" s="11">
+        <v>200</v>
+      </c>
+      <c r="M4" s="11">
+        <v>400</v>
+      </c>
+      <c r="N4" s="12" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A5" s="5" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C2" s="1" t="s">
+      <c r="B5" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="F5" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="N5" s="7" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A6" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="B6" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="C6" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D6" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="F6" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="G6" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="H6" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="I6" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="J6" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="K6" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="L6" s="6">
+        <v>200</v>
+      </c>
+      <c r="M6" s="6">
+        <v>400</v>
+      </c>
+      <c r="N6" s="7" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="D7" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E2" t="s">
-        <v>24</v>
-      </c>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
-      <c r="H2" s="5"/>
-      <c r="I2" s="5"/>
-      <c r="N2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="3" spans="1:20" s="9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="B3" s="8"/>
-      <c r="C3" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" s="8" t="s">
+      <c r="E7" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="N7" s="7" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="D8" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="F3" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="G3" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="H3" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="I3" s="10"/>
-      <c r="J3" s="11" t="s">
-        <v>45</v>
-      </c>
-      <c r="K3" s="11"/>
-      <c r="L3" s="8">
-        <v>201</v>
-      </c>
-      <c r="M3" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="N3" s="9" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E4" t="s">
-        <v>33</v>
-      </c>
-      <c r="G4" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="N4" t="s">
+      <c r="E8" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="N8" s="7" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A5" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="B5" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E5" t="s">
-        <v>27</v>
-      </c>
-      <c r="F5" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="N5" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="6" spans="1:20" s="14" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="12" t="s">
-        <v>53</v>
-      </c>
-      <c r="B6" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="C6" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="D6" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="E6" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="F6" s="15" t="s">
-        <v>44</v>
-      </c>
-      <c r="G6" s="15" t="s">
-        <v>44</v>
-      </c>
-      <c r="H6" s="15" t="s">
-        <v>45</v>
-      </c>
-      <c r="I6" s="15" t="s">
-        <v>54</v>
-      </c>
-      <c r="J6" s="16" t="b">
-        <v>1</v>
-      </c>
-      <c r="K6" s="16" t="s">
-        <v>57</v>
-      </c>
-      <c r="L6" s="13">
-        <v>200</v>
-      </c>
-      <c r="M6" s="13">
-        <v>400</v>
-      </c>
-      <c r="N6" s="14" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="D7" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E7" t="s">
-        <v>24</v>
-      </c>
-      <c r="N7" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="D8" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E8" t="s">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A9" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="N8" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A9" s="2" t="s">
+      <c r="C9" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="E9" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="C9" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E9" t="s">
+      <c r="H9" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="J9" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="L9" s="6">
+        <v>204</v>
+      </c>
+      <c r="M9" s="6">
+        <v>404</v>
+      </c>
+      <c r="N9" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="H9" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="J9" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="L9" s="1">
-        <v>204</v>
-      </c>
-      <c r="M9" s="1">
-        <v>404</v>
-      </c>
-      <c r="N9" t="s">
-        <v>42</v>
-      </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:N11">
-    <sortCondition ref="N2:N11"/>
-    <sortCondition ref="E2:E11"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:N10">
+    <sortCondition ref="N2:N10"/>
+    <sortCondition ref="E2:E10"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15B428E4-A42D-3B45-BCA1-500850D8D31F}">
+  <dimension ref="A3:K16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="H16" sqref="H16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="31.6640625" customWidth="1"/>
+    <col min="5" max="8" width="18.83203125" customWidth="1"/>
+    <col min="9" max="11" width="10.83203125" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:11" s="2" customFormat="1" ht="68" x14ac:dyDescent="0.2">
+      <c r="E3" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B4" t="s">
+        <v>58</v>
+      </c>
+      <c r="C4">
+        <v>40</v>
+      </c>
+      <c r="D4" t="s">
+        <v>59</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B5" t="s">
+        <v>58</v>
+      </c>
+      <c r="C5">
+        <v>20</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B6" t="s">
+        <v>58</v>
+      </c>
+      <c r="C6">
+        <v>15</v>
+      </c>
+      <c r="D6" t="s">
+        <v>64</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B7" t="s">
+        <v>65</v>
+      </c>
+      <c r="C7">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B8" t="s">
+        <v>65</v>
+      </c>
+      <c r="C8">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B9" t="s">
+        <v>65</v>
+      </c>
+      <c r="C9">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B10" t="s">
+        <v>65</v>
+      </c>
+      <c r="C10">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>66</v>
+      </c>
+      <c r="B11" t="s">
+        <v>58</v>
+      </c>
+      <c r="C11">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>60</v>
+      </c>
+      <c r="B12" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>60</v>
+      </c>
+      <c r="B13" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B15" t="s">
+        <v>38</v>
+      </c>
+      <c r="C15">
+        <v>45</v>
+      </c>
+      <c r="E15" t="s">
+        <v>71</v>
+      </c>
+      <c r="F15" t="s">
+        <v>71</v>
+      </c>
+      <c r="G15" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B16" t="s">
+        <v>38</v>
+      </c>
+      <c r="F16" t="s">
+        <v>71</v>
+      </c>
+      <c r="H16" t="s">
+        <v>71</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>